<commit_message>
added test for dir argument
</commit_message>
<xml_diff>
--- a/tests/testthat/test_data/test_df.xlsx
+++ b/tests/testthat/test_data/test_df.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - test_df" sheetId="1" r:id="rId4"/>
+    <sheet name="abc" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -47,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -59,13 +59,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -84,8 +89,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -97,6 +108,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -110,7 +143,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -119,7 +152,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -128,43 +161,28 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -173,28 +191,58 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -204,41 +252,47 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -258,8 +312,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -278,10 +334,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -458,11 +514,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -471,7 +530,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -486,12 +545,12 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -748,10 +807,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1042,7 +1101,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1323,7 +1382,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E152"/>
+  <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1341,2575 +1400,2575 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+      <c r="A2" t="s" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" t="s" s="5">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" t="s" s="5">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" t="s" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="4">
+      <c r="A3" s="6">
         <v>5.1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="7">
         <v>3.5</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="8">
         <v>1.4</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="8">
         <v>0.2</v>
       </c>
-      <c r="E3" t="s" s="7">
+      <c r="E3" t="s" s="9">
         <v>6</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="8">
+      <c r="A4" s="10">
         <v>4.9</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="11">
         <v>3</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="12">
         <v>1.4</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="12">
         <v>0.2</v>
       </c>
-      <c r="E4" t="s" s="11">
+      <c r="E4" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="8">
+      <c r="A5" s="10">
         <v>4.7</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="11">
         <v>3.2</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="12">
         <v>1.3</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="12">
         <v>0.2</v>
       </c>
-      <c r="E5" t="s" s="11">
+      <c r="E5" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="8">
+      <c r="A6" s="10">
         <v>4.6</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="11">
         <v>3.1</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="12">
         <v>1.5</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="12">
         <v>0.2</v>
       </c>
-      <c r="E6" t="s" s="11">
+      <c r="E6" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="8">
+      <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="11">
         <v>3.6</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="12">
         <v>1.4</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="12">
         <v>0.2</v>
       </c>
-      <c r="E7" t="s" s="11">
+      <c r="E7" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="8">
+      <c r="A8" s="10">
         <v>5.4</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="11">
         <v>3.9</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="12">
         <v>1.7</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="12">
         <v>0.4</v>
       </c>
-      <c r="E8" t="s" s="11">
+      <c r="E8" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="8">
+      <c r="A9" s="10">
         <v>4.6</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="11">
         <v>3.4</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="12">
         <v>1.4</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="12">
         <v>0.3</v>
       </c>
-      <c r="E9" t="s" s="11">
+      <c r="E9" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="8">
+      <c r="A10" s="10">
         <v>5</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="11">
         <v>3.4</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="12">
         <v>1.5</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="12">
         <v>0.2</v>
       </c>
-      <c r="E10" t="s" s="11">
+      <c r="E10" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="8">
+      <c r="A11" s="10">
         <v>4.4</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="11">
         <v>2.9</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="12">
         <v>1.4</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="12">
         <v>0.2</v>
       </c>
-      <c r="E11" t="s" s="11">
+      <c r="E11" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="8">
+      <c r="A12" s="10">
         <v>4.9</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="11">
         <v>3.1</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="12">
         <v>1.5</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="12">
         <v>0.1</v>
       </c>
-      <c r="E12" t="s" s="11">
+      <c r="E12" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="8">
+      <c r="A13" s="10">
         <v>5.4</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="11">
         <v>3.7</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="12">
         <v>1.5</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="12">
         <v>0.2</v>
       </c>
-      <c r="E13" t="s" s="11">
+      <c r="E13" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="8">
+      <c r="A14" s="10">
         <v>4.8</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="11">
         <v>3.4</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="12">
         <v>1.6</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="12">
         <v>0.2</v>
       </c>
-      <c r="E14" t="s" s="11">
+      <c r="E14" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="8">
+      <c r="A15" s="10">
         <v>4.8</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="11">
         <v>3</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="12">
         <v>1.4</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="12">
         <v>0.1</v>
       </c>
-      <c r="E15" t="s" s="11">
+      <c r="E15" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="8">
+      <c r="A16" s="10">
         <v>4.3</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="11">
         <v>3</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="12">
         <v>1.1</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="12">
         <v>0.1</v>
       </c>
-      <c r="E16" t="s" s="11">
+      <c r="E16" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="8">
+      <c r="A17" s="10">
         <v>5.8</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="11">
         <v>4</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="12">
         <v>1.2</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="12">
         <v>0.2</v>
       </c>
-      <c r="E17" t="s" s="11">
+      <c r="E17" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="8">
+      <c r="A18" s="10">
         <v>5.7</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="11">
         <v>4.4</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="12">
         <v>1.5</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="12">
         <v>0.4</v>
       </c>
-      <c r="E18" t="s" s="11">
+      <c r="E18" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="8">
+      <c r="A19" s="10">
         <v>5.4</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="11">
         <v>3.9</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="12">
         <v>1.3</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="12">
         <v>0.4</v>
       </c>
-      <c r="E19" t="s" s="11">
+      <c r="E19" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="8">
+      <c r="A20" s="10">
         <v>5.1</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="11">
         <v>3.5</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="12">
         <v>1.4</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="12">
         <v>0.3</v>
       </c>
-      <c r="E20" t="s" s="11">
+      <c r="E20" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="8">
+      <c r="A21" s="10">
         <v>5.7</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="11">
         <v>3.8</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="12">
         <v>1.7</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="12">
         <v>0.3</v>
       </c>
-      <c r="E21" t="s" s="11">
+      <c r="E21" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="8">
+      <c r="A22" s="10">
         <v>5.1</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="11">
         <v>3.8</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="12">
         <v>1.5</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="12">
         <v>0.3</v>
       </c>
-      <c r="E22" t="s" s="11">
+      <c r="E22" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="8">
+      <c r="A23" s="10">
         <v>5.4</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="11">
         <v>3.4</v>
       </c>
-      <c r="C23" s="10">
+      <c r="C23" s="12">
         <v>1.7</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="12">
         <v>0.2</v>
       </c>
-      <c r="E23" t="s" s="11">
+      <c r="E23" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" s="8">
+      <c r="A24" s="10">
         <v>5.1</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="11">
         <v>3.7</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="12">
         <v>1.5</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="12">
         <v>0.4</v>
       </c>
-      <c r="E24" t="s" s="11">
+      <c r="E24" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
-      <c r="A25" s="8">
+      <c r="A25" s="10">
         <v>4.6</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="11">
         <v>3.6</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="12">
         <v>1</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="12">
         <v>0.2</v>
       </c>
-      <c r="E25" t="s" s="11">
+      <c r="E25" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
-      <c r="A26" s="8">
+      <c r="A26" s="10">
         <v>5.1</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="11">
         <v>3.3</v>
       </c>
-      <c r="C26" s="10">
+      <c r="C26" s="12">
         <v>1.7</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="12">
         <v>0.5</v>
       </c>
-      <c r="E26" t="s" s="11">
+      <c r="E26" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
-      <c r="A27" s="8">
+      <c r="A27" s="10">
         <v>4.8</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="11">
         <v>3.4</v>
       </c>
-      <c r="C27" s="10">
+      <c r="C27" s="12">
         <v>1.9</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D27" s="12">
         <v>0.2</v>
       </c>
-      <c r="E27" t="s" s="11">
+      <c r="E27" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="28" ht="20.05" customHeight="1">
-      <c r="A28" s="8">
+      <c r="A28" s="10">
         <v>5</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="11">
         <v>3</v>
       </c>
-      <c r="C28" s="10">
+      <c r="C28" s="12">
         <v>1.6</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="12">
         <v>0.2</v>
       </c>
-      <c r="E28" t="s" s="11">
+      <c r="E28" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="29" ht="20.05" customHeight="1">
-      <c r="A29" s="8">
+      <c r="A29" s="10">
         <v>5</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="11">
         <v>3.4</v>
       </c>
-      <c r="C29" s="10">
+      <c r="C29" s="12">
         <v>1.6</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="12">
         <v>0.4</v>
       </c>
-      <c r="E29" t="s" s="11">
+      <c r="E29" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
-      <c r="A30" s="8">
+      <c r="A30" s="10">
         <v>5.2</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="11">
         <v>3.5</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C30" s="12">
         <v>1.5</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D30" s="12">
         <v>0.2</v>
       </c>
-      <c r="E30" t="s" s="11">
+      <c r="E30" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="31" ht="20.05" customHeight="1">
-      <c r="A31" s="8">
+      <c r="A31" s="10">
         <v>5.2</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="11">
         <v>3.4</v>
       </c>
-      <c r="C31" s="10">
+      <c r="C31" s="12">
         <v>1.4</v>
       </c>
-      <c r="D31" s="10">
+      <c r="D31" s="12">
         <v>0.2</v>
       </c>
-      <c r="E31" t="s" s="11">
+      <c r="E31" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="32" ht="20.05" customHeight="1">
-      <c r="A32" s="8">
+      <c r="A32" s="10">
         <v>4.7</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="11">
         <v>3.2</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="12">
         <v>1.6</v>
       </c>
-      <c r="D32" s="10">
+      <c r="D32" s="12">
         <v>0.2</v>
       </c>
-      <c r="E32" t="s" s="11">
+      <c r="E32" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="33" ht="20.05" customHeight="1">
-      <c r="A33" s="8">
+      <c r="A33" s="10">
         <v>4.8</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="11">
         <v>3.1</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="12">
         <v>1.6</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="12">
         <v>0.2</v>
       </c>
-      <c r="E33" t="s" s="11">
+      <c r="E33" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="34" ht="20.05" customHeight="1">
-      <c r="A34" s="8">
+      <c r="A34" s="10">
         <v>5.4</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="11">
         <v>3.4</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="12">
         <v>1.5</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="12">
         <v>0.4</v>
       </c>
-      <c r="E34" t="s" s="11">
+      <c r="E34" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="35" ht="20.05" customHeight="1">
-      <c r="A35" s="8">
+      <c r="A35" s="10">
         <v>5.2</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="11">
         <v>4.1</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="12">
         <v>1.5</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="12">
         <v>0.1</v>
       </c>
-      <c r="E35" t="s" s="11">
+      <c r="E35" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="36" ht="20.05" customHeight="1">
-      <c r="A36" s="8">
+      <c r="A36" s="10">
         <v>5.5</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="11">
         <v>4.2</v>
       </c>
-      <c r="C36" s="10">
+      <c r="C36" s="12">
         <v>1.4</v>
       </c>
-      <c r="D36" s="10">
+      <c r="D36" s="12">
         <v>0.2</v>
       </c>
-      <c r="E36" t="s" s="11">
+      <c r="E36" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="37" ht="20.05" customHeight="1">
-      <c r="A37" s="8">
+      <c r="A37" s="10">
         <v>4.9</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="11">
         <v>3.1</v>
       </c>
-      <c r="C37" s="10">
+      <c r="C37" s="12">
         <v>1.5</v>
       </c>
-      <c r="D37" s="10">
+      <c r="D37" s="12">
         <v>0.2</v>
       </c>
-      <c r="E37" t="s" s="11">
+      <c r="E37" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="38" ht="20.05" customHeight="1">
-      <c r="A38" s="8">
+      <c r="A38" s="10">
         <v>5</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="11">
         <v>3.2</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="12">
         <v>1.2</v>
       </c>
-      <c r="D38" s="10">
+      <c r="D38" s="12">
         <v>0.2</v>
       </c>
-      <c r="E38" t="s" s="11">
+      <c r="E38" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="39" ht="20.05" customHeight="1">
-      <c r="A39" s="8">
+      <c r="A39" s="10">
         <v>5.5</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="11">
         <v>3.5</v>
       </c>
-      <c r="C39" s="10">
+      <c r="C39" s="12">
         <v>1.3</v>
       </c>
-      <c r="D39" s="10">
+      <c r="D39" s="12">
         <v>0.2</v>
       </c>
-      <c r="E39" t="s" s="11">
+      <c r="E39" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="40" ht="20.05" customHeight="1">
-      <c r="A40" s="8">
+      <c r="A40" s="10">
         <v>4.9</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="11">
         <v>3.6</v>
       </c>
-      <c r="C40" s="10">
+      <c r="C40" s="12">
         <v>1.4</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="12">
         <v>0.1</v>
       </c>
-      <c r="E40" t="s" s="11">
+      <c r="E40" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
-      <c r="A41" s="8">
+      <c r="A41" s="10">
         <v>4.4</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="11">
         <v>3</v>
       </c>
-      <c r="C41" s="10">
+      <c r="C41" s="12">
         <v>1.3</v>
       </c>
-      <c r="D41" s="10">
+      <c r="D41" s="12">
         <v>0.2</v>
       </c>
-      <c r="E41" t="s" s="11">
+      <c r="E41" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="42" ht="20.05" customHeight="1">
-      <c r="A42" s="8">
+      <c r="A42" s="10">
         <v>5.1</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="11">
         <v>3.4</v>
       </c>
-      <c r="C42" s="10">
+      <c r="C42" s="12">
         <v>1.5</v>
       </c>
-      <c r="D42" s="10">
+      <c r="D42" s="12">
         <v>0.2</v>
       </c>
-      <c r="E42" t="s" s="11">
+      <c r="E42" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="43" ht="20.05" customHeight="1">
-      <c r="A43" s="8">
+      <c r="A43" s="10">
         <v>5</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="11">
         <v>3.5</v>
       </c>
-      <c r="C43" s="10">
+      <c r="C43" s="12">
         <v>1.3</v>
       </c>
-      <c r="D43" s="10">
+      <c r="D43" s="12">
         <v>0.3</v>
       </c>
-      <c r="E43" t="s" s="11">
+      <c r="E43" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="44" ht="20.05" customHeight="1">
-      <c r="A44" s="8">
+      <c r="A44" s="10">
         <v>4.5</v>
       </c>
-      <c r="B44" s="9">
+      <c r="B44" s="11">
         <v>2.3</v>
       </c>
-      <c r="C44" s="10">
+      <c r="C44" s="12">
         <v>1.3</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="12">
         <v>0.3</v>
       </c>
-      <c r="E44" t="s" s="11">
+      <c r="E44" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="45" ht="20.05" customHeight="1">
-      <c r="A45" s="8">
+      <c r="A45" s="10">
         <v>4.4</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="11">
         <v>3.2</v>
       </c>
-      <c r="C45" s="10">
+      <c r="C45" s="12">
         <v>1.3</v>
       </c>
-      <c r="D45" s="10">
+      <c r="D45" s="12">
         <v>0.2</v>
       </c>
-      <c r="E45" t="s" s="11">
+      <c r="E45" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="46" ht="20.05" customHeight="1">
-      <c r="A46" s="8">
+      <c r="A46" s="10">
         <v>5</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="11">
         <v>3.5</v>
       </c>
-      <c r="C46" s="10">
+      <c r="C46" s="12">
         <v>1.6</v>
       </c>
-      <c r="D46" s="10">
+      <c r="D46" s="12">
         <v>0.6</v>
       </c>
-      <c r="E46" t="s" s="11">
+      <c r="E46" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="47" ht="20.05" customHeight="1">
-      <c r="A47" s="8">
+      <c r="A47" s="10">
         <v>5.1</v>
       </c>
-      <c r="B47" s="9">
+      <c r="B47" s="11">
         <v>3.8</v>
       </c>
-      <c r="C47" s="10">
+      <c r="C47" s="12">
         <v>1.9</v>
       </c>
-      <c r="D47" s="10">
+      <c r="D47" s="12">
         <v>0.4</v>
       </c>
-      <c r="E47" t="s" s="11">
+      <c r="E47" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="48" ht="20.05" customHeight="1">
-      <c r="A48" s="8">
+      <c r="A48" s="10">
         <v>4.8</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48" s="11">
         <v>3</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C48" s="12">
         <v>1.4</v>
       </c>
-      <c r="D48" s="10">
+      <c r="D48" s="12">
         <v>0.3</v>
       </c>
-      <c r="E48" t="s" s="11">
+      <c r="E48" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="49" ht="20.05" customHeight="1">
-      <c r="A49" s="8">
+      <c r="A49" s="10">
         <v>5.1</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B49" s="11">
         <v>3.8</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C49" s="12">
         <v>1.6</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D49" s="12">
         <v>0.2</v>
       </c>
-      <c r="E49" t="s" s="11">
+      <c r="E49" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="50" ht="20.05" customHeight="1">
-      <c r="A50" s="8">
+      <c r="A50" s="10">
         <v>4.6</v>
       </c>
-      <c r="B50" s="9">
+      <c r="B50" s="11">
         <v>3.2</v>
       </c>
-      <c r="C50" s="10">
+      <c r="C50" s="12">
         <v>1.4</v>
       </c>
-      <c r="D50" s="10">
+      <c r="D50" s="12">
         <v>0.2</v>
       </c>
-      <c r="E50" t="s" s="11">
+      <c r="E50" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="51" ht="20.05" customHeight="1">
-      <c r="A51" s="8">
+      <c r="A51" s="10">
         <v>5.3</v>
       </c>
-      <c r="B51" s="9">
+      <c r="B51" s="11">
         <v>3.7</v>
       </c>
-      <c r="C51" s="10">
+      <c r="C51" s="12">
         <v>1.5</v>
       </c>
-      <c r="D51" s="10">
+      <c r="D51" s="12">
         <v>0.2</v>
       </c>
-      <c r="E51" t="s" s="11">
+      <c r="E51" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="52" ht="20.05" customHeight="1">
-      <c r="A52" s="8">
+      <c r="A52" s="10">
         <v>5</v>
       </c>
-      <c r="B52" s="9">
+      <c r="B52" s="11">
         <v>3.3</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C52" s="12">
         <v>1.4</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D52" s="12">
         <v>0.2</v>
       </c>
-      <c r="E52" t="s" s="11">
+      <c r="E52" t="s" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="53" ht="20.05" customHeight="1">
-      <c r="A53" s="8">
-        <v>7</v>
-      </c>
-      <c r="B53" s="9">
+      <c r="A53" s="10">
+        <v>7</v>
+      </c>
+      <c r="B53" s="11">
         <v>3.2</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C53" s="12">
         <v>4.7</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D53" s="12">
         <v>1.4</v>
       </c>
-      <c r="E53" t="s" s="11">
+      <c r="E53" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="54" ht="20.05" customHeight="1">
-      <c r="A54" s="8">
+      <c r="A54" s="10">
         <v>6.4</v>
       </c>
-      <c r="B54" s="9">
+      <c r="B54" s="11">
         <v>3.2</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C54" s="12">
         <v>4.5</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D54" s="12">
         <v>1.5</v>
       </c>
-      <c r="E54" t="s" s="11">
+      <c r="E54" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="55" ht="20.05" customHeight="1">
-      <c r="A55" s="8">
+      <c r="A55" s="10">
         <v>6.9</v>
       </c>
-      <c r="B55" s="9">
+      <c r="B55" s="11">
         <v>3.1</v>
       </c>
-      <c r="C55" s="10">
+      <c r="C55" s="12">
         <v>4.9</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D55" s="12">
         <v>1.5</v>
       </c>
-      <c r="E55" t="s" s="11">
+      <c r="E55" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="56" ht="20.05" customHeight="1">
-      <c r="A56" s="8">
+      <c r="A56" s="10">
         <v>5.5</v>
       </c>
-      <c r="B56" s="9">
+      <c r="B56" s="11">
         <v>2.3</v>
       </c>
-      <c r="C56" s="10">
+      <c r="C56" s="12">
         <v>4</v>
       </c>
-      <c r="D56" s="10">
+      <c r="D56" s="12">
         <v>1.3</v>
       </c>
-      <c r="E56" t="s" s="11">
+      <c r="E56" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="57" ht="20.05" customHeight="1">
-      <c r="A57" s="8">
+      <c r="A57" s="10">
         <v>6.5</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B57" s="11">
         <v>2.8</v>
       </c>
-      <c r="C57" s="10">
+      <c r="C57" s="12">
         <v>4.6</v>
       </c>
-      <c r="D57" s="10">
+      <c r="D57" s="12">
         <v>1.5</v>
       </c>
-      <c r="E57" t="s" s="11">
+      <c r="E57" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="58" ht="20.05" customHeight="1">
-      <c r="A58" s="8">
+      <c r="A58" s="10">
         <v>5.7</v>
       </c>
-      <c r="B58" s="9">
+      <c r="B58" s="11">
         <v>2.8</v>
       </c>
-      <c r="C58" s="10">
+      <c r="C58" s="12">
         <v>4.5</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="12">
         <v>1.3</v>
       </c>
-      <c r="E58" t="s" s="11">
+      <c r="E58" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="59" ht="20.05" customHeight="1">
-      <c r="A59" s="8">
+      <c r="A59" s="10">
         <v>6.3</v>
       </c>
-      <c r="B59" s="9">
+      <c r="B59" s="11">
         <v>3.3</v>
       </c>
-      <c r="C59" s="10">
+      <c r="C59" s="12">
         <v>4.7</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="12">
         <v>1.6</v>
       </c>
-      <c r="E59" t="s" s="11">
+      <c r="E59" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="60" ht="20.05" customHeight="1">
-      <c r="A60" s="8">
+      <c r="A60" s="10">
         <v>4.9</v>
       </c>
-      <c r="B60" s="9">
+      <c r="B60" s="11">
         <v>2.4</v>
       </c>
-      <c r="C60" s="10">
+      <c r="C60" s="12">
         <v>3.3</v>
       </c>
-      <c r="D60" s="10">
+      <c r="D60" s="12">
         <v>1</v>
       </c>
-      <c r="E60" t="s" s="11">
+      <c r="E60" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="61" ht="20.05" customHeight="1">
-      <c r="A61" s="8">
+      <c r="A61" s="10">
         <v>6.6</v>
       </c>
-      <c r="B61" s="9">
+      <c r="B61" s="11">
         <v>2.9</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C61" s="12">
         <v>4.6</v>
       </c>
-      <c r="D61" s="10">
+      <c r="D61" s="12">
         <v>1.3</v>
       </c>
-      <c r="E61" t="s" s="11">
+      <c r="E61" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="62" ht="20.05" customHeight="1">
-      <c r="A62" s="8">
+      <c r="A62" s="10">
         <v>5.2</v>
       </c>
-      <c r="B62" s="9">
+      <c r="B62" s="11">
         <v>2.7</v>
       </c>
-      <c r="C62" s="10">
+      <c r="C62" s="12">
         <v>3.9</v>
       </c>
-      <c r="D62" s="10">
+      <c r="D62" s="12">
         <v>1.4</v>
       </c>
-      <c r="E62" t="s" s="11">
+      <c r="E62" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="63" ht="20.05" customHeight="1">
-      <c r="A63" s="8">
+      <c r="A63" s="10">
         <v>5</v>
       </c>
-      <c r="B63" s="9">
+      <c r="B63" s="11">
         <v>2</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="12">
         <v>3.5</v>
       </c>
-      <c r="D63" s="10">
+      <c r="D63" s="12">
         <v>1</v>
       </c>
-      <c r="E63" t="s" s="11">
+      <c r="E63" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="64" ht="20.05" customHeight="1">
-      <c r="A64" s="8">
+      <c r="A64" s="10">
         <v>5.9</v>
       </c>
-      <c r="B64" s="9">
+      <c r="B64" s="11">
         <v>3</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C64" s="12">
         <v>4.2</v>
       </c>
-      <c r="D64" s="10">
+      <c r="D64" s="12">
         <v>1.5</v>
       </c>
-      <c r="E64" t="s" s="11">
+      <c r="E64" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="65" ht="20.05" customHeight="1">
-      <c r="A65" s="8">
-        <v>6</v>
-      </c>
-      <c r="B65" s="9">
+      <c r="A65" s="10">
+        <v>6</v>
+      </c>
+      <c r="B65" s="11">
         <v>2.2</v>
       </c>
-      <c r="C65" s="10">
+      <c r="C65" s="12">
         <v>4</v>
       </c>
-      <c r="D65" s="10">
+      <c r="D65" s="12">
         <v>1</v>
       </c>
-      <c r="E65" t="s" s="11">
+      <c r="E65" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="66" ht="20.05" customHeight="1">
-      <c r="A66" s="8">
+      <c r="A66" s="10">
         <v>6.1</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B66" s="11">
         <v>2.9</v>
       </c>
-      <c r="C66" s="10">
+      <c r="C66" s="12">
         <v>4.7</v>
       </c>
-      <c r="D66" s="10">
+      <c r="D66" s="12">
         <v>1.4</v>
       </c>
-      <c r="E66" t="s" s="11">
+      <c r="E66" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="67" ht="20.05" customHeight="1">
-      <c r="A67" s="8">
+      <c r="A67" s="10">
         <v>5.6</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B67" s="11">
         <v>2.9</v>
       </c>
-      <c r="C67" s="10">
+      <c r="C67" s="12">
         <v>3.6</v>
       </c>
-      <c r="D67" s="10">
+      <c r="D67" s="12">
         <v>1.3</v>
       </c>
-      <c r="E67" t="s" s="11">
+      <c r="E67" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="68" ht="20.05" customHeight="1">
-      <c r="A68" s="8">
+      <c r="A68" s="10">
         <v>6.7</v>
       </c>
-      <c r="B68" s="9">
+      <c r="B68" s="11">
         <v>3.1</v>
       </c>
-      <c r="C68" s="10">
+      <c r="C68" s="12">
         <v>4.4</v>
       </c>
-      <c r="D68" s="10">
+      <c r="D68" s="12">
         <v>1.4</v>
       </c>
-      <c r="E68" t="s" s="11">
+      <c r="E68" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="69" ht="20.05" customHeight="1">
-      <c r="A69" s="8">
+      <c r="A69" s="10">
         <v>5.6</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="11">
         <v>3</v>
       </c>
-      <c r="C69" s="10">
+      <c r="C69" s="12">
         <v>4.5</v>
       </c>
-      <c r="D69" s="10">
+      <c r="D69" s="12">
         <v>1.5</v>
       </c>
-      <c r="E69" t="s" s="11">
+      <c r="E69" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="70" ht="20.05" customHeight="1">
-      <c r="A70" s="8">
+      <c r="A70" s="10">
         <v>5.8</v>
       </c>
-      <c r="B70" s="9">
+      <c r="B70" s="11">
         <v>2.7</v>
       </c>
-      <c r="C70" s="10">
+      <c r="C70" s="12">
         <v>4.1</v>
       </c>
-      <c r="D70" s="10">
+      <c r="D70" s="12">
         <v>1</v>
       </c>
-      <c r="E70" t="s" s="11">
+      <c r="E70" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="71" ht="20.05" customHeight="1">
-      <c r="A71" s="8">
+      <c r="A71" s="10">
         <v>6.2</v>
       </c>
-      <c r="B71" s="9">
+      <c r="B71" s="11">
         <v>2.2</v>
       </c>
-      <c r="C71" s="10">
+      <c r="C71" s="12">
         <v>4.5</v>
       </c>
-      <c r="D71" s="10">
+      <c r="D71" s="12">
         <v>1.5</v>
       </c>
-      <c r="E71" t="s" s="11">
+      <c r="E71" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="72" ht="20.05" customHeight="1">
-      <c r="A72" s="8">
+      <c r="A72" s="10">
         <v>5.6</v>
       </c>
-      <c r="B72" s="9">
+      <c r="B72" s="11">
         <v>2.5</v>
       </c>
-      <c r="C72" s="10">
+      <c r="C72" s="12">
         <v>3.9</v>
       </c>
-      <c r="D72" s="10">
+      <c r="D72" s="12">
         <v>1.1</v>
       </c>
-      <c r="E72" t="s" s="11">
+      <c r="E72" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="73" ht="20.05" customHeight="1">
-      <c r="A73" s="8">
+      <c r="A73" s="10">
         <v>5.9</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B73" s="11">
         <v>3.2</v>
       </c>
-      <c r="C73" s="10">
+      <c r="C73" s="12">
         <v>4.8</v>
       </c>
-      <c r="D73" s="10">
+      <c r="D73" s="12">
         <v>1.8</v>
       </c>
-      <c r="E73" t="s" s="11">
+      <c r="E73" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="74" ht="20.05" customHeight="1">
-      <c r="A74" s="8">
+      <c r="A74" s="10">
         <v>6.1</v>
       </c>
-      <c r="B74" s="9">
+      <c r="B74" s="11">
         <v>2.8</v>
       </c>
-      <c r="C74" s="10">
+      <c r="C74" s="12">
         <v>4</v>
       </c>
-      <c r="D74" s="10">
+      <c r="D74" s="12">
         <v>1.3</v>
       </c>
-      <c r="E74" t="s" s="11">
+      <c r="E74" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="75" ht="20.05" customHeight="1">
-      <c r="A75" s="8">
+      <c r="A75" s="10">
         <v>6.3</v>
       </c>
-      <c r="B75" s="9">
+      <c r="B75" s="11">
         <v>2.5</v>
       </c>
-      <c r="C75" s="10">
+      <c r="C75" s="12">
         <v>4.9</v>
       </c>
-      <c r="D75" s="10">
+      <c r="D75" s="12">
         <v>1.5</v>
       </c>
-      <c r="E75" t="s" s="11">
+      <c r="E75" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="76" ht="20.05" customHeight="1">
-      <c r="A76" s="8">
+      <c r="A76" s="10">
         <v>6.1</v>
       </c>
-      <c r="B76" s="9">
+      <c r="B76" s="11">
         <v>2.8</v>
       </c>
-      <c r="C76" s="10">
+      <c r="C76" s="12">
         <v>4.7</v>
       </c>
-      <c r="D76" s="10">
+      <c r="D76" s="12">
         <v>1.2</v>
       </c>
-      <c r="E76" t="s" s="11">
+      <c r="E76" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="77" ht="20.05" customHeight="1">
-      <c r="A77" s="8">
+      <c r="A77" s="10">
         <v>6.4</v>
       </c>
-      <c r="B77" s="9">
+      <c r="B77" s="11">
         <v>2.9</v>
       </c>
-      <c r="C77" s="10">
+      <c r="C77" s="12">
         <v>4.3</v>
       </c>
-      <c r="D77" s="10">
+      <c r="D77" s="12">
         <v>1.3</v>
       </c>
-      <c r="E77" t="s" s="11">
+      <c r="E77" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="78" ht="20.05" customHeight="1">
-      <c r="A78" s="8">
+      <c r="A78" s="10">
         <v>6.6</v>
       </c>
-      <c r="B78" s="9">
+      <c r="B78" s="11">
         <v>3</v>
       </c>
-      <c r="C78" s="10">
+      <c r="C78" s="12">
         <v>4.4</v>
       </c>
-      <c r="D78" s="10">
+      <c r="D78" s="12">
         <v>1.4</v>
       </c>
-      <c r="E78" t="s" s="11">
+      <c r="E78" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="79" ht="20.05" customHeight="1">
-      <c r="A79" s="8">
+      <c r="A79" s="10">
         <v>6.8</v>
       </c>
-      <c r="B79" s="9">
+      <c r="B79" s="11">
         <v>2.8</v>
       </c>
-      <c r="C79" s="10">
+      <c r="C79" s="12">
         <v>4.8</v>
       </c>
-      <c r="D79" s="10">
+      <c r="D79" s="12">
         <v>1.4</v>
       </c>
-      <c r="E79" t="s" s="11">
+      <c r="E79" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="80" ht="20.05" customHeight="1">
-      <c r="A80" s="8">
+      <c r="A80" s="10">
         <v>6.7</v>
       </c>
-      <c r="B80" s="9">
+      <c r="B80" s="11">
         <v>3</v>
       </c>
-      <c r="C80" s="10">
+      <c r="C80" s="12">
         <v>5</v>
       </c>
-      <c r="D80" s="10">
+      <c r="D80" s="12">
         <v>1.7</v>
       </c>
-      <c r="E80" t="s" s="11">
+      <c r="E80" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="81" ht="20.05" customHeight="1">
-      <c r="A81" s="8">
-        <v>6</v>
-      </c>
-      <c r="B81" s="9">
+      <c r="A81" s="10">
+        <v>6</v>
+      </c>
+      <c r="B81" s="11">
         <v>2.9</v>
       </c>
-      <c r="C81" s="10">
+      <c r="C81" s="12">
         <v>4.5</v>
       </c>
-      <c r="D81" s="10">
+      <c r="D81" s="12">
         <v>1.5</v>
       </c>
-      <c r="E81" t="s" s="11">
+      <c r="E81" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="82" ht="20.05" customHeight="1">
-      <c r="A82" s="8">
+      <c r="A82" s="10">
         <v>5.7</v>
       </c>
-      <c r="B82" s="9">
+      <c r="B82" s="11">
         <v>2.6</v>
       </c>
-      <c r="C82" s="10">
+      <c r="C82" s="12">
         <v>3.5</v>
       </c>
-      <c r="D82" s="10">
+      <c r="D82" s="12">
         <v>1</v>
       </c>
-      <c r="E82" t="s" s="11">
+      <c r="E82" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="83" ht="20.05" customHeight="1">
-      <c r="A83" s="8">
+      <c r="A83" s="10">
         <v>5.5</v>
       </c>
-      <c r="B83" s="9">
+      <c r="B83" s="11">
         <v>2.4</v>
       </c>
-      <c r="C83" s="10">
+      <c r="C83" s="12">
         <v>3.8</v>
       </c>
-      <c r="D83" s="10">
+      <c r="D83" s="12">
         <v>1.1</v>
       </c>
-      <c r="E83" t="s" s="11">
+      <c r="E83" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="84" ht="20.05" customHeight="1">
-      <c r="A84" s="8">
+      <c r="A84" s="10">
         <v>5.5</v>
       </c>
-      <c r="B84" s="9">
+      <c r="B84" s="11">
         <v>2.4</v>
       </c>
-      <c r="C84" s="10">
+      <c r="C84" s="12">
         <v>3.7</v>
       </c>
-      <c r="D84" s="10">
+      <c r="D84" s="12">
         <v>1</v>
       </c>
-      <c r="E84" t="s" s="11">
+      <c r="E84" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="85" ht="20.05" customHeight="1">
-      <c r="A85" s="8">
+      <c r="A85" s="10">
         <v>5.8</v>
       </c>
-      <c r="B85" s="9">
+      <c r="B85" s="11">
         <v>2.7</v>
       </c>
-      <c r="C85" s="10">
+      <c r="C85" s="12">
         <v>3.9</v>
       </c>
-      <c r="D85" s="10">
+      <c r="D85" s="12">
         <v>1.2</v>
       </c>
-      <c r="E85" t="s" s="11">
+      <c r="E85" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="86" ht="20.05" customHeight="1">
-      <c r="A86" s="8">
-        <v>6</v>
-      </c>
-      <c r="B86" s="9">
+      <c r="A86" s="10">
+        <v>6</v>
+      </c>
+      <c r="B86" s="11">
         <v>2.7</v>
       </c>
-      <c r="C86" s="10">
+      <c r="C86" s="12">
         <v>5.1</v>
       </c>
-      <c r="D86" s="10">
+      <c r="D86" s="12">
         <v>1.6</v>
       </c>
-      <c r="E86" t="s" s="11">
+      <c r="E86" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="87" ht="20.05" customHeight="1">
-      <c r="A87" s="8">
+      <c r="A87" s="10">
         <v>5.4</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B87" s="11">
         <v>3</v>
       </c>
-      <c r="C87" s="10">
+      <c r="C87" s="12">
         <v>4.5</v>
       </c>
-      <c r="D87" s="10">
+      <c r="D87" s="12">
         <v>1.5</v>
       </c>
-      <c r="E87" t="s" s="11">
+      <c r="E87" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="88" ht="20.05" customHeight="1">
-      <c r="A88" s="8">
-        <v>6</v>
-      </c>
-      <c r="B88" s="9">
+      <c r="A88" s="10">
+        <v>6</v>
+      </c>
+      <c r="B88" s="11">
         <v>3.4</v>
       </c>
-      <c r="C88" s="10">
+      <c r="C88" s="12">
         <v>4.5</v>
       </c>
-      <c r="D88" s="10">
+      <c r="D88" s="12">
         <v>1.6</v>
       </c>
-      <c r="E88" t="s" s="11">
+      <c r="E88" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="89" ht="20.05" customHeight="1">
-      <c r="A89" s="8">
+      <c r="A89" s="10">
         <v>6.7</v>
       </c>
-      <c r="B89" s="9">
+      <c r="B89" s="11">
         <v>3.1</v>
       </c>
-      <c r="C89" s="10">
+      <c r="C89" s="12">
         <v>4.7</v>
       </c>
-      <c r="D89" s="10">
+      <c r="D89" s="12">
         <v>1.5</v>
       </c>
-      <c r="E89" t="s" s="11">
+      <c r="E89" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="90" ht="20.05" customHeight="1">
-      <c r="A90" s="8">
+      <c r="A90" s="10">
         <v>6.3</v>
       </c>
-      <c r="B90" s="9">
+      <c r="B90" s="11">
         <v>2.3</v>
       </c>
-      <c r="C90" s="10">
+      <c r="C90" s="12">
         <v>4.4</v>
       </c>
-      <c r="D90" s="10">
+      <c r="D90" s="12">
         <v>1.3</v>
       </c>
-      <c r="E90" t="s" s="11">
+      <c r="E90" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="91" ht="20.05" customHeight="1">
-      <c r="A91" s="8">
+      <c r="A91" s="10">
         <v>5.6</v>
       </c>
-      <c r="B91" s="9">
+      <c r="B91" s="11">
         <v>3</v>
       </c>
-      <c r="C91" s="10">
+      <c r="C91" s="12">
         <v>4.1</v>
       </c>
-      <c r="D91" s="10">
+      <c r="D91" s="12">
         <v>1.3</v>
       </c>
-      <c r="E91" t="s" s="11">
+      <c r="E91" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="92" ht="20.05" customHeight="1">
-      <c r="A92" s="8">
+      <c r="A92" s="10">
         <v>5.5</v>
       </c>
-      <c r="B92" s="9">
+      <c r="B92" s="11">
         <v>2.5</v>
       </c>
-      <c r="C92" s="10">
+      <c r="C92" s="12">
         <v>4</v>
       </c>
-      <c r="D92" s="10">
+      <c r="D92" s="12">
         <v>1.3</v>
       </c>
-      <c r="E92" t="s" s="11">
+      <c r="E92" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="93" ht="20.05" customHeight="1">
-      <c r="A93" s="8">
+      <c r="A93" s="10">
         <v>5.5</v>
       </c>
-      <c r="B93" s="9">
+      <c r="B93" s="11">
         <v>2.6</v>
       </c>
-      <c r="C93" s="10">
+      <c r="C93" s="12">
         <v>4.4</v>
       </c>
-      <c r="D93" s="10">
+      <c r="D93" s="12">
         <v>1.2</v>
       </c>
-      <c r="E93" t="s" s="11">
+      <c r="E93" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="94" ht="20.05" customHeight="1">
-      <c r="A94" s="8">
+      <c r="A94" s="10">
         <v>6.1</v>
       </c>
-      <c r="B94" s="9">
+      <c r="B94" s="11">
         <v>3</v>
       </c>
-      <c r="C94" s="10">
+      <c r="C94" s="12">
         <v>4.6</v>
       </c>
-      <c r="D94" s="10">
+      <c r="D94" s="12">
         <v>1.4</v>
       </c>
-      <c r="E94" t="s" s="11">
+      <c r="E94" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="95" ht="20.05" customHeight="1">
-      <c r="A95" s="8">
+      <c r="A95" s="10">
         <v>5.8</v>
       </c>
-      <c r="B95" s="9">
+      <c r="B95" s="11">
         <v>2.6</v>
       </c>
-      <c r="C95" s="10">
+      <c r="C95" s="12">
         <v>4</v>
       </c>
-      <c r="D95" s="10">
+      <c r="D95" s="12">
         <v>1.2</v>
       </c>
-      <c r="E95" t="s" s="11">
+      <c r="E95" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="96" ht="20.05" customHeight="1">
-      <c r="A96" s="8">
+      <c r="A96" s="10">
         <v>5</v>
       </c>
-      <c r="B96" s="9">
+      <c r="B96" s="11">
         <v>2.3</v>
       </c>
-      <c r="C96" s="10">
+      <c r="C96" s="12">
         <v>3.3</v>
       </c>
-      <c r="D96" s="10">
+      <c r="D96" s="12">
         <v>1</v>
       </c>
-      <c r="E96" t="s" s="11">
+      <c r="E96" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="97" ht="20.05" customHeight="1">
-      <c r="A97" s="8">
+      <c r="A97" s="10">
         <v>5.6</v>
       </c>
-      <c r="B97" s="9">
+      <c r="B97" s="11">
         <v>2.7</v>
       </c>
-      <c r="C97" s="10">
+      <c r="C97" s="12">
         <v>4.2</v>
       </c>
-      <c r="D97" s="10">
+      <c r="D97" s="12">
         <v>1.3</v>
       </c>
-      <c r="E97" t="s" s="11">
+      <c r="E97" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="98" ht="20.05" customHeight="1">
-      <c r="A98" s="8">
+      <c r="A98" s="10">
         <v>5.7</v>
       </c>
-      <c r="B98" s="9">
+      <c r="B98" s="11">
         <v>3</v>
       </c>
-      <c r="C98" s="10">
+      <c r="C98" s="12">
         <v>4.2</v>
       </c>
-      <c r="D98" s="10">
+      <c r="D98" s="12">
         <v>1.2</v>
       </c>
-      <c r="E98" t="s" s="11">
+      <c r="E98" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="99" ht="20.05" customHeight="1">
-      <c r="A99" s="8">
+      <c r="A99" s="10">
         <v>5.7</v>
       </c>
-      <c r="B99" s="9">
+      <c r="B99" s="11">
         <v>2.9</v>
       </c>
-      <c r="C99" s="10">
+      <c r="C99" s="12">
         <v>4.2</v>
       </c>
-      <c r="D99" s="10">
+      <c r="D99" s="12">
         <v>1.3</v>
       </c>
-      <c r="E99" t="s" s="11">
+      <c r="E99" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="100" ht="20.05" customHeight="1">
-      <c r="A100" s="8">
+      <c r="A100" s="10">
         <v>6.2</v>
       </c>
-      <c r="B100" s="9">
+      <c r="B100" s="11">
         <v>2.9</v>
       </c>
-      <c r="C100" s="10">
+      <c r="C100" s="12">
         <v>4.3</v>
       </c>
-      <c r="D100" s="10">
+      <c r="D100" s="12">
         <v>1.3</v>
       </c>
-      <c r="E100" t="s" s="11">
+      <c r="E100" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="101" ht="20.05" customHeight="1">
-      <c r="A101" s="8">
+      <c r="A101" s="10">
         <v>5.1</v>
       </c>
-      <c r="B101" s="9">
+      <c r="B101" s="11">
         <v>2.5</v>
       </c>
-      <c r="C101" s="10">
+      <c r="C101" s="12">
         <v>3</v>
       </c>
-      <c r="D101" s="10">
+      <c r="D101" s="12">
         <v>1.1</v>
       </c>
-      <c r="E101" t="s" s="11">
+      <c r="E101" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="102" ht="20.05" customHeight="1">
-      <c r="A102" s="8">
+      <c r="A102" s="10">
         <v>5.7</v>
       </c>
-      <c r="B102" s="9">
+      <c r="B102" s="11">
         <v>2.8</v>
       </c>
-      <c r="C102" s="10">
+      <c r="C102" s="12">
         <v>4.1</v>
       </c>
-      <c r="D102" s="10">
+      <c r="D102" s="12">
         <v>1.3</v>
       </c>
-      <c r="E102" t="s" s="11">
+      <c r="E102" t="s" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="103" ht="20.05" customHeight="1">
-      <c r="A103" s="8">
+      <c r="A103" s="10">
         <v>6.3</v>
       </c>
-      <c r="B103" s="9">
+      <c r="B103" s="11">
         <v>3.3</v>
       </c>
-      <c r="C103" s="10">
-        <v>6</v>
-      </c>
-      <c r="D103" s="10">
+      <c r="C103" s="12">
+        <v>6</v>
+      </c>
+      <c r="D103" s="12">
         <v>2.5</v>
       </c>
-      <c r="E103" t="s" s="11">
+      <c r="E103" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="104" ht="20.05" customHeight="1">
-      <c r="A104" s="8">
+      <c r="A104" s="10">
         <v>5.8</v>
       </c>
-      <c r="B104" s="9">
+      <c r="B104" s="11">
         <v>2.7</v>
       </c>
-      <c r="C104" s="10">
+      <c r="C104" s="12">
         <v>5.1</v>
       </c>
-      <c r="D104" s="10">
+      <c r="D104" s="12">
         <v>1.9</v>
       </c>
-      <c r="E104" t="s" s="11">
+      <c r="E104" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="105" ht="20.05" customHeight="1">
-      <c r="A105" s="8">
+      <c r="A105" s="10">
         <v>7.1</v>
       </c>
-      <c r="B105" s="9">
+      <c r="B105" s="11">
         <v>3</v>
       </c>
-      <c r="C105" s="10">
+      <c r="C105" s="12">
         <v>5.9</v>
       </c>
-      <c r="D105" s="10">
+      <c r="D105" s="12">
         <v>2.1</v>
       </c>
-      <c r="E105" t="s" s="11">
+      <c r="E105" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="106" ht="20.05" customHeight="1">
-      <c r="A106" s="8">
+      <c r="A106" s="10">
         <v>6.3</v>
       </c>
-      <c r="B106" s="9">
+      <c r="B106" s="11">
         <v>2.9</v>
       </c>
-      <c r="C106" s="10">
+      <c r="C106" s="12">
         <v>5.6</v>
       </c>
-      <c r="D106" s="10">
+      <c r="D106" s="12">
         <v>1.8</v>
       </c>
-      <c r="E106" t="s" s="11">
+      <c r="E106" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="107" ht="20.05" customHeight="1">
-      <c r="A107" s="8">
+      <c r="A107" s="10">
         <v>6.5</v>
       </c>
-      <c r="B107" s="9">
+      <c r="B107" s="11">
         <v>3</v>
       </c>
-      <c r="C107" s="10">
+      <c r="C107" s="12">
         <v>5.8</v>
       </c>
-      <c r="D107" s="10">
+      <c r="D107" s="12">
         <v>2.2</v>
       </c>
-      <c r="E107" t="s" s="11">
+      <c r="E107" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="108" ht="20.05" customHeight="1">
-      <c r="A108" s="8">
+      <c r="A108" s="10">
         <v>7.6</v>
       </c>
-      <c r="B108" s="9">
+      <c r="B108" s="11">
         <v>3</v>
       </c>
-      <c r="C108" s="10">
+      <c r="C108" s="12">
         <v>6.6</v>
       </c>
-      <c r="D108" s="10">
+      <c r="D108" s="12">
         <v>2.1</v>
       </c>
-      <c r="E108" t="s" s="11">
+      <c r="E108" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="109" ht="20.05" customHeight="1">
-      <c r="A109" s="8">
+      <c r="A109" s="10">
         <v>4.9</v>
       </c>
-      <c r="B109" s="9">
+      <c r="B109" s="11">
         <v>2.5</v>
       </c>
-      <c r="C109" s="10">
+      <c r="C109" s="12">
         <v>4.5</v>
       </c>
-      <c r="D109" s="10">
+      <c r="D109" s="12">
         <v>1.7</v>
       </c>
-      <c r="E109" t="s" s="11">
+      <c r="E109" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="110" ht="20.05" customHeight="1">
-      <c r="A110" s="8">
+      <c r="A110" s="10">
         <v>7.3</v>
       </c>
-      <c r="B110" s="9">
+      <c r="B110" s="11">
         <v>2.9</v>
       </c>
-      <c r="C110" s="10">
+      <c r="C110" s="12">
         <v>6.3</v>
       </c>
-      <c r="D110" s="10">
+      <c r="D110" s="12">
         <v>1.8</v>
       </c>
-      <c r="E110" t="s" s="11">
+      <c r="E110" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="111" ht="20.05" customHeight="1">
-      <c r="A111" s="8">
+      <c r="A111" s="10">
         <v>6.7</v>
       </c>
-      <c r="B111" s="9">
+      <c r="B111" s="11">
         <v>2.5</v>
       </c>
-      <c r="C111" s="10">
+      <c r="C111" s="12">
         <v>5.8</v>
       </c>
-      <c r="D111" s="10">
+      <c r="D111" s="12">
         <v>1.8</v>
       </c>
-      <c r="E111" t="s" s="11">
+      <c r="E111" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="112" ht="20.05" customHeight="1">
-      <c r="A112" s="8">
+      <c r="A112" s="10">
         <v>7.2</v>
       </c>
-      <c r="B112" s="9">
+      <c r="B112" s="11">
         <v>3.6</v>
       </c>
-      <c r="C112" s="10">
+      <c r="C112" s="12">
         <v>6.1</v>
       </c>
-      <c r="D112" s="10">
+      <c r="D112" s="12">
         <v>2.5</v>
       </c>
-      <c r="E112" t="s" s="11">
+      <c r="E112" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="113" ht="20.05" customHeight="1">
-      <c r="A113" s="8">
+      <c r="A113" s="10">
         <v>6.5</v>
       </c>
-      <c r="B113" s="9">
+      <c r="B113" s="11">
         <v>3.2</v>
       </c>
-      <c r="C113" s="10">
+      <c r="C113" s="12">
         <v>5.1</v>
       </c>
-      <c r="D113" s="10">
+      <c r="D113" s="12">
         <v>2</v>
       </c>
-      <c r="E113" t="s" s="11">
+      <c r="E113" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="114" ht="20.05" customHeight="1">
-      <c r="A114" s="8">
+      <c r="A114" s="10">
         <v>6.4</v>
       </c>
-      <c r="B114" s="9">
+      <c r="B114" s="11">
         <v>2.7</v>
       </c>
-      <c r="C114" s="10">
+      <c r="C114" s="12">
         <v>5.3</v>
       </c>
-      <c r="D114" s="10">
+      <c r="D114" s="12">
         <v>1.9</v>
       </c>
-      <c r="E114" t="s" s="11">
+      <c r="E114" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="115" ht="20.05" customHeight="1">
-      <c r="A115" s="8">
+      <c r="A115" s="10">
         <v>6.8</v>
       </c>
-      <c r="B115" s="9">
+      <c r="B115" s="11">
         <v>3</v>
       </c>
-      <c r="C115" s="10">
+      <c r="C115" s="12">
         <v>5.5</v>
       </c>
-      <c r="D115" s="10">
+      <c r="D115" s="12">
         <v>2.1</v>
       </c>
-      <c r="E115" t="s" s="11">
+      <c r="E115" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="116" ht="20.05" customHeight="1">
-      <c r="A116" s="8">
+      <c r="A116" s="10">
         <v>5.7</v>
       </c>
-      <c r="B116" s="9">
+      <c r="B116" s="11">
         <v>2.5</v>
       </c>
-      <c r="C116" s="10">
+      <c r="C116" s="12">
         <v>5</v>
       </c>
-      <c r="D116" s="10">
+      <c r="D116" s="12">
         <v>2</v>
       </c>
-      <c r="E116" t="s" s="11">
+      <c r="E116" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="117" ht="20.05" customHeight="1">
-      <c r="A117" s="8">
+      <c r="A117" s="10">
         <v>5.8</v>
       </c>
-      <c r="B117" s="9">
+      <c r="B117" s="11">
         <v>2.8</v>
       </c>
-      <c r="C117" s="10">
+      <c r="C117" s="12">
         <v>5.1</v>
       </c>
-      <c r="D117" s="10">
+      <c r="D117" s="12">
         <v>2.4</v>
       </c>
-      <c r="E117" t="s" s="11">
+      <c r="E117" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="118" ht="20.05" customHeight="1">
-      <c r="A118" s="8">
+      <c r="A118" s="10">
         <v>6.4</v>
       </c>
-      <c r="B118" s="9">
+      <c r="B118" s="11">
         <v>3.2</v>
       </c>
-      <c r="C118" s="10">
+      <c r="C118" s="12">
         <v>5.3</v>
       </c>
-      <c r="D118" s="10">
+      <c r="D118" s="12">
         <v>2.3</v>
       </c>
-      <c r="E118" t="s" s="11">
+      <c r="E118" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="119" ht="20.05" customHeight="1">
-      <c r="A119" s="8">
+      <c r="A119" s="10">
         <v>6.5</v>
       </c>
-      <c r="B119" s="9">
+      <c r="B119" s="11">
         <v>3</v>
       </c>
-      <c r="C119" s="10">
+      <c r="C119" s="12">
         <v>5.5</v>
       </c>
-      <c r="D119" s="10">
+      <c r="D119" s="12">
         <v>1.8</v>
       </c>
-      <c r="E119" t="s" s="11">
+      <c r="E119" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="120" ht="20.05" customHeight="1">
-      <c r="A120" s="8">
+      <c r="A120" s="10">
         <v>7.7</v>
       </c>
-      <c r="B120" s="9">
+      <c r="B120" s="11">
         <v>3.8</v>
       </c>
-      <c r="C120" s="10">
+      <c r="C120" s="12">
         <v>6.7</v>
       </c>
-      <c r="D120" s="10">
+      <c r="D120" s="12">
         <v>2.2</v>
       </c>
-      <c r="E120" t="s" s="11">
+      <c r="E120" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="121" ht="20.05" customHeight="1">
-      <c r="A121" s="8">
+      <c r="A121" s="10">
         <v>7.7</v>
       </c>
-      <c r="B121" s="9">
+      <c r="B121" s="11">
         <v>2.6</v>
       </c>
-      <c r="C121" s="10">
+      <c r="C121" s="12">
         <v>6.9</v>
       </c>
-      <c r="D121" s="10">
+      <c r="D121" s="12">
         <v>2.3</v>
       </c>
-      <c r="E121" t="s" s="11">
+      <c r="E121" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="122" ht="20.05" customHeight="1">
-      <c r="A122" s="8">
-        <v>6</v>
-      </c>
-      <c r="B122" s="9">
+      <c r="A122" s="10">
+        <v>6</v>
+      </c>
+      <c r="B122" s="11">
         <v>2.2</v>
       </c>
-      <c r="C122" s="10">
+      <c r="C122" s="12">
         <v>5</v>
       </c>
-      <c r="D122" s="10">
+      <c r="D122" s="12">
         <v>1.5</v>
       </c>
-      <c r="E122" t="s" s="11">
+      <c r="E122" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="123" ht="20.05" customHeight="1">
-      <c r="A123" s="8">
+      <c r="A123" s="10">
         <v>6.9</v>
       </c>
-      <c r="B123" s="9">
+      <c r="B123" s="11">
         <v>3.2</v>
       </c>
-      <c r="C123" s="10">
+      <c r="C123" s="12">
         <v>5.7</v>
       </c>
-      <c r="D123" s="10">
+      <c r="D123" s="12">
         <v>2.3</v>
       </c>
-      <c r="E123" t="s" s="11">
+      <c r="E123" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="124" ht="20.05" customHeight="1">
-      <c r="A124" s="8">
+      <c r="A124" s="10">
         <v>5.6</v>
       </c>
-      <c r="B124" s="9">
+      <c r="B124" s="11">
         <v>2.8</v>
       </c>
-      <c r="C124" s="10">
+      <c r="C124" s="12">
         <v>4.9</v>
       </c>
-      <c r="D124" s="10">
+      <c r="D124" s="12">
         <v>2</v>
       </c>
-      <c r="E124" t="s" s="11">
+      <c r="E124" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="125" ht="20.05" customHeight="1">
-      <c r="A125" s="8">
+      <c r="A125" s="10">
         <v>7.7</v>
       </c>
-      <c r="B125" s="9">
+      <c r="B125" s="11">
         <v>2.8</v>
       </c>
-      <c r="C125" s="10">
+      <c r="C125" s="12">
         <v>6.7</v>
       </c>
-      <c r="D125" s="10">
+      <c r="D125" s="12">
         <v>2</v>
       </c>
-      <c r="E125" t="s" s="11">
+      <c r="E125" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="126" ht="20.05" customHeight="1">
-      <c r="A126" s="8">
+      <c r="A126" s="10">
         <v>6.3</v>
       </c>
-      <c r="B126" s="9">
+      <c r="B126" s="11">
         <v>2.7</v>
       </c>
-      <c r="C126" s="10">
+      <c r="C126" s="12">
         <v>4.9</v>
       </c>
-      <c r="D126" s="10">
+      <c r="D126" s="12">
         <v>1.8</v>
       </c>
-      <c r="E126" t="s" s="11">
+      <c r="E126" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="127" ht="20.05" customHeight="1">
-      <c r="A127" s="8">
+      <c r="A127" s="10">
         <v>6.7</v>
       </c>
-      <c r="B127" s="9">
+      <c r="B127" s="11">
         <v>3.3</v>
       </c>
-      <c r="C127" s="10">
+      <c r="C127" s="12">
         <v>5.7</v>
       </c>
-      <c r="D127" s="10">
+      <c r="D127" s="12">
         <v>2.1</v>
       </c>
-      <c r="E127" t="s" s="11">
+      <c r="E127" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="128" ht="20.05" customHeight="1">
-      <c r="A128" s="8">
+      <c r="A128" s="10">
         <v>7.2</v>
       </c>
-      <c r="B128" s="9">
+      <c r="B128" s="11">
         <v>3.2</v>
       </c>
-      <c r="C128" s="10">
-        <v>6</v>
-      </c>
-      <c r="D128" s="10">
+      <c r="C128" s="12">
+        <v>6</v>
+      </c>
+      <c r="D128" s="12">
         <v>1.8</v>
       </c>
-      <c r="E128" t="s" s="11">
+      <c r="E128" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="129" ht="20.05" customHeight="1">
-      <c r="A129" s="8">
+      <c r="A129" s="10">
         <v>6.2</v>
       </c>
-      <c r="B129" s="9">
+      <c r="B129" s="11">
         <v>2.8</v>
       </c>
-      <c r="C129" s="10">
+      <c r="C129" s="12">
         <v>4.8</v>
       </c>
-      <c r="D129" s="10">
+      <c r="D129" s="12">
         <v>1.8</v>
       </c>
-      <c r="E129" t="s" s="11">
+      <c r="E129" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="130" ht="20.05" customHeight="1">
-      <c r="A130" s="8">
+      <c r="A130" s="10">
         <v>6.1</v>
       </c>
-      <c r="B130" s="9">
+      <c r="B130" s="11">
         <v>3</v>
       </c>
-      <c r="C130" s="10">
+      <c r="C130" s="12">
         <v>4.9</v>
       </c>
-      <c r="D130" s="10">
+      <c r="D130" s="12">
         <v>1.8</v>
       </c>
-      <c r="E130" t="s" s="11">
+      <c r="E130" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="131" ht="20.05" customHeight="1">
-      <c r="A131" s="8">
+      <c r="A131" s="10">
         <v>6.4</v>
       </c>
-      <c r="B131" s="9">
+      <c r="B131" s="11">
         <v>2.8</v>
       </c>
-      <c r="C131" s="10">
+      <c r="C131" s="12">
         <v>5.6</v>
       </c>
-      <c r="D131" s="10">
+      <c r="D131" s="12">
         <v>2.1</v>
       </c>
-      <c r="E131" t="s" s="11">
+      <c r="E131" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="132" ht="20.05" customHeight="1">
-      <c r="A132" s="8">
+      <c r="A132" s="10">
         <v>7.2</v>
       </c>
-      <c r="B132" s="9">
+      <c r="B132" s="11">
         <v>3</v>
       </c>
-      <c r="C132" s="10">
+      <c r="C132" s="12">
         <v>5.8</v>
       </c>
-      <c r="D132" s="10">
+      <c r="D132" s="12">
         <v>1.6</v>
       </c>
-      <c r="E132" t="s" s="11">
+      <c r="E132" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="133" ht="20.05" customHeight="1">
-      <c r="A133" s="8">
+      <c r="A133" s="10">
         <v>7.4</v>
       </c>
-      <c r="B133" s="9">
+      <c r="B133" s="11">
         <v>2.8</v>
       </c>
-      <c r="C133" s="10">
+      <c r="C133" s="12">
         <v>6.1</v>
       </c>
-      <c r="D133" s="10">
+      <c r="D133" s="12">
         <v>1.9</v>
       </c>
-      <c r="E133" t="s" s="11">
+      <c r="E133" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="134" ht="20.05" customHeight="1">
-      <c r="A134" s="8">
+      <c r="A134" s="10">
         <v>7.9</v>
       </c>
-      <c r="B134" s="9">
+      <c r="B134" s="11">
         <v>3.8</v>
       </c>
-      <c r="C134" s="10">
+      <c r="C134" s="12">
         <v>6.4</v>
       </c>
-      <c r="D134" s="10">
+      <c r="D134" s="12">
         <v>2</v>
       </c>
-      <c r="E134" t="s" s="11">
+      <c r="E134" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="135" ht="20.05" customHeight="1">
-      <c r="A135" s="8">
+      <c r="A135" s="10">
         <v>6.4</v>
       </c>
-      <c r="B135" s="9">
+      <c r="B135" s="11">
         <v>2.8</v>
       </c>
-      <c r="C135" s="10">
+      <c r="C135" s="12">
         <v>5.6</v>
       </c>
-      <c r="D135" s="10">
+      <c r="D135" s="12">
         <v>2.2</v>
       </c>
-      <c r="E135" t="s" s="11">
+      <c r="E135" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="136" ht="20.05" customHeight="1">
-      <c r="A136" s="8">
+      <c r="A136" s="10">
         <v>6.3</v>
       </c>
-      <c r="B136" s="9">
+      <c r="B136" s="11">
         <v>2.8</v>
       </c>
-      <c r="C136" s="10">
+      <c r="C136" s="12">
         <v>5.1</v>
       </c>
-      <c r="D136" s="10">
+      <c r="D136" s="12">
         <v>1.5</v>
       </c>
-      <c r="E136" t="s" s="11">
+      <c r="E136" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="137" ht="20.05" customHeight="1">
-      <c r="A137" s="8">
+      <c r="A137" s="10">
         <v>6.1</v>
       </c>
-      <c r="B137" s="9">
+      <c r="B137" s="11">
         <v>2.6</v>
       </c>
-      <c r="C137" s="10">
+      <c r="C137" s="12">
         <v>5.6</v>
       </c>
-      <c r="D137" s="10">
+      <c r="D137" s="12">
         <v>1.4</v>
       </c>
-      <c r="E137" t="s" s="11">
+      <c r="E137" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="138" ht="20.05" customHeight="1">
-      <c r="A138" s="8">
+      <c r="A138" s="10">
         <v>7.7</v>
       </c>
-      <c r="B138" s="9">
+      <c r="B138" s="11">
         <v>3</v>
       </c>
-      <c r="C138" s="10">
+      <c r="C138" s="12">
         <v>6.1</v>
       </c>
-      <c r="D138" s="10">
+      <c r="D138" s="12">
         <v>2.3</v>
       </c>
-      <c r="E138" t="s" s="11">
+      <c r="E138" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="139" ht="20.05" customHeight="1">
-      <c r="A139" s="8">
+      <c r="A139" s="10">
         <v>6.3</v>
       </c>
-      <c r="B139" s="9">
+      <c r="B139" s="11">
         <v>3.4</v>
       </c>
-      <c r="C139" s="10">
+      <c r="C139" s="12">
         <v>5.6</v>
       </c>
-      <c r="D139" s="10">
+      <c r="D139" s="12">
         <v>2.4</v>
       </c>
-      <c r="E139" t="s" s="11">
+      <c r="E139" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="140" ht="20.05" customHeight="1">
-      <c r="A140" s="8">
+      <c r="A140" s="10">
         <v>6.4</v>
       </c>
-      <c r="B140" s="9">
+      <c r="B140" s="11">
         <v>3.1</v>
       </c>
-      <c r="C140" s="10">
+      <c r="C140" s="12">
         <v>5.5</v>
       </c>
-      <c r="D140" s="10">
+      <c r="D140" s="12">
         <v>1.8</v>
       </c>
-      <c r="E140" t="s" s="11">
+      <c r="E140" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="141" ht="20.05" customHeight="1">
-      <c r="A141" s="8">
-        <v>6</v>
-      </c>
-      <c r="B141" s="9">
+      <c r="A141" s="10">
+        <v>6</v>
+      </c>
+      <c r="B141" s="11">
         <v>3</v>
       </c>
-      <c r="C141" s="10">
+      <c r="C141" s="12">
         <v>4.8</v>
       </c>
-      <c r="D141" s="10">
+      <c r="D141" s="12">
         <v>1.8</v>
       </c>
-      <c r="E141" t="s" s="11">
+      <c r="E141" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="142" ht="20.05" customHeight="1">
-      <c r="A142" s="8">
+      <c r="A142" s="10">
         <v>6.9</v>
       </c>
-      <c r="B142" s="9">
+      <c r="B142" s="11">
         <v>3.1</v>
       </c>
-      <c r="C142" s="10">
+      <c r="C142" s="12">
         <v>5.4</v>
       </c>
-      <c r="D142" s="10">
+      <c r="D142" s="12">
         <v>2.1</v>
       </c>
-      <c r="E142" t="s" s="11">
+      <c r="E142" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="143" ht="20.05" customHeight="1">
-      <c r="A143" s="8">
+      <c r="A143" s="10">
         <v>6.7</v>
       </c>
-      <c r="B143" s="9">
+      <c r="B143" s="11">
         <v>3.1</v>
       </c>
-      <c r="C143" s="10">
+      <c r="C143" s="12">
         <v>5.6</v>
       </c>
-      <c r="D143" s="10">
+      <c r="D143" s="12">
         <v>2.4</v>
       </c>
-      <c r="E143" t="s" s="11">
+      <c r="E143" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="144" ht="20.05" customHeight="1">
-      <c r="A144" s="8">
+      <c r="A144" s="10">
         <v>6.9</v>
       </c>
-      <c r="B144" s="9">
+      <c r="B144" s="11">
         <v>3.1</v>
       </c>
-      <c r="C144" s="10">
+      <c r="C144" s="12">
         <v>5.1</v>
       </c>
-      <c r="D144" s="10">
+      <c r="D144" s="12">
         <v>2.3</v>
       </c>
-      <c r="E144" t="s" s="11">
+      <c r="E144" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="145" ht="20.05" customHeight="1">
-      <c r="A145" s="8">
+      <c r="A145" s="10">
         <v>5.8</v>
       </c>
-      <c r="B145" s="9">
+      <c r="B145" s="11">
         <v>2.7</v>
       </c>
-      <c r="C145" s="10">
+      <c r="C145" s="12">
         <v>5.1</v>
       </c>
-      <c r="D145" s="10">
+      <c r="D145" s="12">
         <v>1.9</v>
       </c>
-      <c r="E145" t="s" s="11">
+      <c r="E145" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="146" ht="20.05" customHeight="1">
-      <c r="A146" s="8">
+      <c r="A146" s="10">
         <v>6.8</v>
       </c>
-      <c r="B146" s="9">
+      <c r="B146" s="11">
         <v>3.2</v>
       </c>
-      <c r="C146" s="10">
+      <c r="C146" s="12">
         <v>5.9</v>
       </c>
-      <c r="D146" s="10">
+      <c r="D146" s="12">
         <v>2.3</v>
       </c>
-      <c r="E146" t="s" s="11">
+      <c r="E146" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="147" ht="20.05" customHeight="1">
-      <c r="A147" s="8">
+      <c r="A147" s="10">
         <v>6.7</v>
       </c>
-      <c r="B147" s="9">
+      <c r="B147" s="11">
         <v>3.3</v>
       </c>
-      <c r="C147" s="10">
+      <c r="C147" s="12">
         <v>5.7</v>
       </c>
-      <c r="D147" s="10">
+      <c r="D147" s="12">
         <v>2.5</v>
       </c>
-      <c r="E147" t="s" s="11">
+      <c r="E147" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="148" ht="20.05" customHeight="1">
-      <c r="A148" s="8">
+      <c r="A148" s="10">
         <v>6.7</v>
       </c>
-      <c r="B148" s="9">
+      <c r="B148" s="11">
         <v>3</v>
       </c>
-      <c r="C148" s="10">
+      <c r="C148" s="12">
         <v>5.2</v>
       </c>
-      <c r="D148" s="10">
+      <c r="D148" s="12">
         <v>2.3</v>
       </c>
-      <c r="E148" t="s" s="11">
+      <c r="E148" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="149" ht="20.05" customHeight="1">
-      <c r="A149" s="8">
+      <c r="A149" s="10">
         <v>6.3</v>
       </c>
-      <c r="B149" s="9">
+      <c r="B149" s="11">
         <v>2.5</v>
       </c>
-      <c r="C149" s="10">
+      <c r="C149" s="12">
         <v>5</v>
       </c>
-      <c r="D149" s="10">
+      <c r="D149" s="12">
         <v>1.9</v>
       </c>
-      <c r="E149" t="s" s="11">
+      <c r="E149" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="150" ht="20.05" customHeight="1">
-      <c r="A150" s="8">
+      <c r="A150" s="10">
         <v>6.5</v>
       </c>
-      <c r="B150" s="9">
+      <c r="B150" s="11">
         <v>3</v>
       </c>
-      <c r="C150" s="10">
+      <c r="C150" s="12">
         <v>5.2</v>
       </c>
-      <c r="D150" s="10">
+      <c r="D150" s="12">
         <v>2</v>
       </c>
-      <c r="E150" t="s" s="11">
+      <c r="E150" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="151" ht="20.05" customHeight="1">
-      <c r="A151" s="8">
+      <c r="A151" s="10">
         <v>6.2</v>
       </c>
-      <c r="B151" s="9">
+      <c r="B151" s="11">
         <v>3.4</v>
       </c>
-      <c r="C151" s="10">
+      <c r="C151" s="12">
         <v>5.4</v>
       </c>
-      <c r="D151" s="10">
+      <c r="D151" s="12">
         <v>2.3</v>
       </c>
-      <c r="E151" t="s" s="11">
+      <c r="E151" t="s" s="13">
         <v>8</v>
       </c>
     </row>
     <row r="152" ht="20.05" customHeight="1">
-      <c r="A152" s="8">
+      <c r="A152" s="10">
         <v>5.9</v>
       </c>
-      <c r="B152" s="9">
+      <c r="B152" s="11">
         <v>3</v>
       </c>
-      <c r="C152" s="10">
+      <c r="C152" s="12">
         <v>5.1</v>
       </c>
-      <c r="D152" s="10">
+      <c r="D152" s="12">
         <v>1.8</v>
       </c>
-      <c r="E152" t="s" s="11">
+      <c r="E152" t="s" s="13">
         <v>8</v>
       </c>
     </row>

</xml_diff>